<commit_message>
testing PM - need to add seconds in then done
</commit_message>
<xml_diff>
--- a/SampleRedBullData.xlsx
+++ b/SampleRedBullData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frankschweitzer/Documents/Emily Cadent/TV_Ad_Scraper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF71559A-A734-2B4C-9CCF-727CE1286960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9557372-8B20-0845-968C-96F67FE0AE8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19240" yWindow="2240" windowWidth="19040" windowHeight="15540" xr2:uid="{321218B8-BE53-BE44-AC05-DF79E6311C27}"/>
+    <workbookView xWindow="-15900" yWindow="1360" windowWidth="19040" windowHeight="15540" xr2:uid="{321218B8-BE53-BE44-AC05-DF79E6311C27}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t>10:31:30 AM</t>
   </si>
   <si>
-    <t>10:50:30 AM</t>
-  </si>
-  <si>
     <t>FX</t>
   </si>
   <si>
@@ -111,6 +108,9 @@
   </si>
   <si>
     <t>5/27/2023</t>
+  </si>
+  <si>
+    <t>10:50:30 PM</t>
   </si>
 </sst>
 </file>
@@ -501,7 +501,7 @@
   <dimension ref="A1:D557"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:D11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -525,13 +525,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -539,13 +539,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -553,7 +553,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>7</v>
@@ -567,13 +567,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -581,13 +581,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -595,7 +595,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>11</v>
@@ -609,13 +609,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -623,13 +623,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -637,13 +637,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>